<commit_message>
Generated Problem Formulation and fixed Excel Solver Solution
</commit_message>
<xml_diff>
--- a/Solution.xlsx
+++ b/Solution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\MSBA-Courses\Fall Semester\Optimization and Simulation - MSBA320\Optimization-Problem\Application 2-Solution+Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\covid19-respirators-OptimizationProblem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A79299-8980-472F-8C54-5C751EEAEEC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B79B4-BDAB-4465-84F5-B431A00F6260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,13 +176,13 @@
     <t>Cost of Yij</t>
   </si>
   <si>
-    <t>equal RHS</t>
-  </si>
-  <si>
-    <t>&lt;= RHS</t>
-  </si>
-  <si>
     <t>Total Cost in LBP</t>
+  </si>
+  <si>
+    <t>Equal Right Hand Side</t>
+  </si>
+  <si>
+    <t>&lt;= Right Hand Side</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>384541</xdr:colOff>
+      <xdr:colOff>384540</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>74931</xdr:rowOff>
     </xdr:to>
@@ -734,7 +734,7 @@
   <dimension ref="A2:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +746,7 @@
     <col min="5" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="2"/>
@@ -1010,7 +1010,7 @@
         <v>36409345.301472038</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
         <v>-5</v>
       </c>
       <c r="L21" s="17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -1147,7 +1147,7 @@
         <v>29</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>